<commit_message>
Changed the excel writer to a pandas df
</commit_message>
<xml_diff>
--- a/mystuff/CardInventory.xlsx
+++ b/mystuff/CardInventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitRepos\pokemon-tcg-data\mystuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F94EFF3-6027-4668-B1C9-B429E60BE952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3975F7E3-8AFC-4AC3-8885-7BAC59BF51A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21990" yWindow="915" windowWidth="21600" windowHeight="11385" xr2:uid="{6AC12905-6D81-4575-9DCC-C58CFC3D361F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{196B95B4-E59E-4896-A860-59A05E3A6BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>PK</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>EBAY_TITLE</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>There needs to be a value in this PK for the pk_calc to work</t>
   </si>
 </sst>
 </file>
@@ -413,22 +419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF9630B-054E-4FE5-89FD-984D09DD62AB}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A62B9B2-7BAE-4C0B-87D7-33738F9FF698}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -457,6 +455,35 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>